<commit_message>
steering training visualization added 🕶
</commit_message>
<xml_diff>
--- a/others/phase-2-shopping-list.xlsx
+++ b/others/phase-2-shopping-list.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yongyangnie/Developer/self-driving-golf-cart/others/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{949AC2CC-3BD3-8640-A6DC-737A6021B59A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C421E5AB-EEC6-AD45-B013-800C06108322}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14360" windowHeight="18000" xr2:uid="{D7D37102-1B4C-444A-B6B6-4E9525F0A280}"/>
+    <workbookView xWindow="1280" yWindow="460" windowWidth="25600" windowHeight="17540" activeTab="1" xr2:uid="{D7D37102-1B4C-444A-B6B6-4E9525F0A280}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="computer" sheetId="1" r:id="rId1"/>
+    <sheet name="other hardware" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="29">
   <si>
     <t>Item</t>
   </si>
@@ -97,6 +98,21 @@
   </si>
   <si>
     <t>Computer Case</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/RioRand-7-80V-Motor-Controller-Switch/dp/B071NQ5G71/ref=sr_1_7?ie=UTF8&amp;qid=1526653434&amp;sr=8-7&amp;keywords=dc+motor+controller</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Motor speed controller</t>
+  </si>
+  <si>
+    <t>High torque DC motor</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/dp/B01N8YDOC9/ref=sspa_dk_detail_1?psc=1</t>
   </si>
 </sst>
 </file>
@@ -450,7 +466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B68760E0-37D1-4F44-996B-98DD21838291}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -731,4 +747,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FF6658A-E10A-F449-BCF3-C36986226238}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2">
+        <v>15.9</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2</f>
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>69</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <f>C3*D3</f>
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>